<commit_message>
Updates for 2019 and 2020 data
Added 2019 and 2020 data for PV installs in the US, and some globally. Reran baseline journals to produce new baselines, copied into baselines and into graphing excels.
To Do: rerun analyses because the market share of silicon vs thinfilm increased based on improved understanding of LBNL data. Make journals more dynamic for annual additions to baselines (i.e. no hard coded years)
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/MaterialCompositionAnnual-Graph.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/MaterialCompositionAnnual-Graph.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEEEC8F-8C1B-405C-AD93-5480EFFEB857}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3229E1F2-B6DA-4A06-8EC7-E9AD68FBD0DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" xr2:uid="{0FB8D6CD-8546-4236-B63D-A974CB21DD58}"/>
+    <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0FB8D6CD-8546-4236-B63D-A974CB21DD58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CSA Scaling" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_ftn1" localSheetId="1">'CSA Scaling'!$A$14</definedName>
+    <definedName name="_ftnref1" localSheetId="1">'CSA Scaling'!$A$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>year</t>
   </si>
@@ -74,15 +79,80 @@
   <si>
     <t>Module Mass [kg] +8% for plastics</t>
   </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>CSA Group</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(437 GW) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[13]</t>
+    </r>
+  </si>
+  <si>
+    <t>CSA Group Scaled</t>
+  </si>
+  <si>
+    <t>(773 GW)</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Polymers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copper[1] </t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>[1] Other material compositions include copper external to the module, including junction box and cabling, while currently our baseline only includes the busbar and cell stringing internal to the module.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -110,16 +180,103 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6235,7 +6392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B855FEC6-71A0-4178-BC01-33F7B8382BFB}">
   <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -9277,4 +9434,230 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14664F1-E6DD-45E9-8C55-1E9289DFBD1B}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.36328125" customWidth="1"/>
+    <col min="2" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D1">
+        <f>777/437</f>
+        <v>1.7780320366132722</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="11"/>
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3">
+        <v>777</v>
+      </c>
+      <c r="E3" s="3">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="8">
+        <v>27000000</v>
+      </c>
+      <c r="C4" s="8">
+        <v>47760000</v>
+      </c>
+      <c r="D4" s="14">
+        <f>B4*$D$1</f>
+        <v>48006864.988558352</v>
+      </c>
+      <c r="E4" s="15">
+        <f>ROUND(D4,-4)</f>
+        <v>48010000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8">
+        <v>20600000</v>
+      </c>
+      <c r="C5" s="8">
+        <v>36440000</v>
+      </c>
+      <c r="D5" s="14">
+        <f t="shared" ref="D5:D11" si="0">B5*$D$1</f>
+        <v>36627459.954233408</v>
+      </c>
+      <c r="E5" s="15">
+        <f t="shared" ref="E5:E11" si="1">ROUND(D5,-4)</f>
+        <v>36630000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2800000</v>
+      </c>
+      <c r="C6" s="7">
+        <v>4950000</v>
+      </c>
+      <c r="D6" s="14">
+        <f t="shared" si="0"/>
+        <v>4978489.7025171621</v>
+      </c>
+      <c r="E6" s="15">
+        <f t="shared" si="1"/>
+        <v>4980000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2100000</v>
+      </c>
+      <c r="C7" s="7">
+        <v>3715000</v>
+      </c>
+      <c r="D7" s="14">
+        <f t="shared" si="0"/>
+        <v>3733867.2768878718</v>
+      </c>
+      <c r="E7" s="15">
+        <f>ROUND(D7,-3)</f>
+        <v>3734000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="8">
+        <v>239000</v>
+      </c>
+      <c r="C8" s="7">
+        <v>423000</v>
+      </c>
+      <c r="D8" s="14">
+        <f t="shared" si="0"/>
+        <v>424949.65675057209</v>
+      </c>
+      <c r="E8" s="15">
+        <f>ROUND(D8,-3)</f>
+        <v>425000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1270000</v>
+      </c>
+      <c r="C9" s="7">
+        <v>2246000</v>
+      </c>
+      <c r="D9" s="14">
+        <f t="shared" si="0"/>
+        <v>2258100.6864988557</v>
+      </c>
+      <c r="E9" s="15">
+        <f>ROUND(D9,-3)</f>
+        <v>2258000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="8">
+        <v>11000</v>
+      </c>
+      <c r="C10" s="7">
+        <v>19000</v>
+      </c>
+      <c r="D10" s="14">
+        <f t="shared" si="0"/>
+        <v>19558.352402745993</v>
+      </c>
+      <c r="E10" s="15">
+        <f>ROUND(D10,-2)</f>
+        <v>19600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="8">
+        <v>170000</v>
+      </c>
+      <c r="C11" s="7">
+        <v>300000</v>
+      </c>
+      <c r="D11" s="14">
+        <f t="shared" si="0"/>
+        <v>302265.4462242563</v>
+      </c>
+      <c r="E11" s="15">
+        <f>ROUND(D11,-2)</f>
+        <v>302300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="12"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A8" location="_ftn1" display="_ftn1" xr:uid="{33F955CD-0490-452F-BCD4-CBAD6472B0BC}"/>
+    <hyperlink ref="A14" location="_ftnref1" display="_ftnref1" xr:uid="{241ABD1F-9ACB-402B-BE02-228EF1684520}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Graph updates, move files
Consolidated graph locations into Harmonize_graphs.xlsx for input to openei
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/MaterialCompositionAnnual-Graph.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/MaterialCompositionAnnual-Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC432B3-E12D-4087-927E-2E34900BFF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB2361E-641B-4634-8C18-A66FAC3FEDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" xr2:uid="{0FB8D6CD-8546-4236-B63D-A974CB21DD58}"/>
   </bookViews>
@@ -9167,7 +9167,7 @@
   <dimension ref="A1:V57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="Y30" sqref="Y30"/>
+      <selection activeCell="AA33" sqref="AA33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated to finished backsheet baseline - weighted for glass marketshare
forgot to weight the final mass by marketshare of glass backsheets, has been corrected in all files now.
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/MaterialCompositionAnnual-Graph.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/MaterialCompositionAnnual-Graph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81F88A0-58E2-4E89-8F70-1A7F3D05DD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B163F7F1-8083-46B6-B6D0-676450FF259F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0FB8D6CD-8546-4236-B63D-A974CB21DD58}"/>
+    <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" xr2:uid="{0FB8D6CD-8546-4236-B63D-A974CB21DD58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6718,172 +6718,172 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
-                  <c:v>532</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>532</c:v>
+                  <c:v>186.48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>532</c:v>
+                  <c:v>192.96</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>532</c:v>
+                  <c:v>199.44</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>532</c:v>
+                  <c:v>205.92</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>532</c:v>
+                  <c:v>212.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>532</c:v>
+                  <c:v>218.88</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>532</c:v>
+                  <c:v>225.36</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>532</c:v>
+                  <c:v>231.84</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>532</c:v>
+                  <c:v>238.0421533</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>532</c:v>
+                  <c:v>244.22710620000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>532</c:v>
+                  <c:v>270.84237130000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>532</c:v>
+                  <c:v>297.39114389999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>532</c:v>
+                  <c:v>323.87268519999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>532</c:v>
+                  <c:v>350.28624539999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>532</c:v>
+                  <c:v>376.63106340000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>532</c:v>
+                  <c:v>402.90636699999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>532</c:v>
+                  <c:v>424.82025850000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>532</c:v>
+                  <c:v>446.14037739999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>532</c:v>
+                  <c:v>450.12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>532</c:v>
+                  <c:v>469.04871969999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>532</c:v>
+                  <c:v>488.55303370000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>532</c:v>
+                  <c:v>480.42291669999997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>532</c:v>
+                  <c:v>472.89833329999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>532</c:v>
+                  <c:v>463.21199999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>532</c:v>
+                  <c:v>432.53280000000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>520</c:v>
+                  <c:v>410.94400000000002</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>510</c:v>
+                  <c:v>400.03859999999997</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>500</c:v>
+                  <c:v>389.16559999999998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>490</c:v>
+                  <c:v>383.15249999999997</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>480</c:v>
+                  <c:v>377.16320000000002</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>470</c:v>
+                  <c:v>362.01006669999998</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>460</c:v>
+                  <c:v>346.84533329999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>450</c:v>
+                  <c:v>331.66899999999998</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>450</c:v>
+                  <c:v>314.73022220000001</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>450</c:v>
+                  <c:v>297.78388890000002</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>450</c:v>
+                  <c:v>280.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9811,8 +9811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B855FEC6-71A0-4178-BC01-33F7B8382BFB}">
   <dimension ref="A1:AH57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="42" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9901,7 +9901,7 @@
         <v>846</v>
       </c>
       <c r="H2">
-        <v>532</v>
+        <v>180</v>
       </c>
       <c r="I2">
         <f>SUM(B2:F2)</f>
@@ -9968,7 +9968,7 @@
         <v>846</v>
       </c>
       <c r="H3">
-        <v>532</v>
+        <v>186.48</v>
       </c>
       <c r="I3">
         <f>SUM(B3:F3)</f>
@@ -10043,7 +10043,7 @@
         <v>846</v>
       </c>
       <c r="H4">
-        <v>532</v>
+        <v>192.96</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I57" si="7">SUM(B4:F4)</f>
@@ -10110,7 +10110,7 @@
         <v>846</v>
       </c>
       <c r="H5">
-        <v>532</v>
+        <v>199.44</v>
       </c>
       <c r="I5">
         <f t="shared" si="7"/>
@@ -10180,7 +10180,7 @@
         <v>846</v>
       </c>
       <c r="H6">
-        <v>532</v>
+        <v>205.92</v>
       </c>
       <c r="I6">
         <f t="shared" si="7"/>
@@ -10248,7 +10248,7 @@
         <v>846</v>
       </c>
       <c r="H7">
-        <v>532</v>
+        <v>212.4</v>
       </c>
       <c r="I7">
         <f t="shared" si="7"/>
@@ -10306,7 +10306,7 @@
         <v>846</v>
       </c>
       <c r="H8">
-        <v>532</v>
+        <v>218.88</v>
       </c>
       <c r="I8">
         <f t="shared" si="7"/>
@@ -10364,7 +10364,7 @@
         <v>846</v>
       </c>
       <c r="H9">
-        <v>532</v>
+        <v>225.36</v>
       </c>
       <c r="I9">
         <f t="shared" si="7"/>
@@ -10422,7 +10422,7 @@
         <v>846</v>
       </c>
       <c r="H10">
-        <v>532</v>
+        <v>231.84</v>
       </c>
       <c r="I10">
         <f t="shared" si="7"/>
@@ -10480,7 +10480,7 @@
         <v>846</v>
       </c>
       <c r="H11">
-        <v>532</v>
+        <v>238.0421533</v>
       </c>
       <c r="I11">
         <f t="shared" si="7"/>
@@ -10538,7 +10538,7 @@
         <v>846</v>
       </c>
       <c r="H12">
-        <v>532</v>
+        <v>244.22710620000001</v>
       </c>
       <c r="I12">
         <f t="shared" si="7"/>
@@ -10596,7 +10596,7 @@
         <v>846</v>
       </c>
       <c r="H13">
-        <v>532</v>
+        <v>270.84237130000002</v>
       </c>
       <c r="I13">
         <f t="shared" si="7"/>
@@ -10654,7 +10654,7 @@
         <v>846</v>
       </c>
       <c r="H14">
-        <v>532</v>
+        <v>297.39114389999997</v>
       </c>
       <c r="I14">
         <f t="shared" si="7"/>
@@ -10712,7 +10712,7 @@
         <v>846</v>
       </c>
       <c r="H15">
-        <v>532</v>
+        <v>323.87268519999998</v>
       </c>
       <c r="I15">
         <f t="shared" si="7"/>
@@ -10770,7 +10770,7 @@
         <v>846</v>
       </c>
       <c r="H16">
-        <v>532</v>
+        <v>350.28624539999998</v>
       </c>
       <c r="I16">
         <f t="shared" si="7"/>
@@ -10828,7 +10828,7 @@
         <v>846</v>
       </c>
       <c r="H17">
-        <v>532</v>
+        <v>376.63106340000002</v>
       </c>
       <c r="I17">
         <f t="shared" si="7"/>
@@ -10886,7 +10886,7 @@
         <v>846</v>
       </c>
       <c r="H18">
-        <v>532</v>
+        <v>402.90636699999999</v>
       </c>
       <c r="I18">
         <f t="shared" si="7"/>
@@ -10944,7 +10944,7 @@
         <v>846</v>
       </c>
       <c r="H19">
-        <v>532</v>
+        <v>424.82025850000002</v>
       </c>
       <c r="I19">
         <f t="shared" si="7"/>
@@ -11002,7 +11002,7 @@
         <v>846</v>
       </c>
       <c r="H20">
-        <v>532</v>
+        <v>446.14037739999998</v>
       </c>
       <c r="I20">
         <f t="shared" si="7"/>
@@ -11060,7 +11060,7 @@
         <v>848.09</v>
       </c>
       <c r="H21">
-        <v>532</v>
+        <v>450.12</v>
       </c>
       <c r="I21">
         <f t="shared" si="7"/>
@@ -11118,7 +11118,7 @@
         <v>850.28</v>
       </c>
       <c r="H22">
-        <v>532</v>
+        <v>469.04871969999999</v>
       </c>
       <c r="I22">
         <f t="shared" si="7"/>
@@ -11176,7 +11176,7 @@
         <v>852.81</v>
       </c>
       <c r="H23">
-        <v>532</v>
+        <v>488.55303370000001</v>
       </c>
       <c r="I23">
         <f t="shared" si="7"/>
@@ -11234,7 +11234,7 @@
         <v>847.99</v>
       </c>
       <c r="H24">
-        <v>532</v>
+        <v>480.42291669999997</v>
       </c>
       <c r="I24">
         <f t="shared" si="7"/>
@@ -11292,7 +11292,7 @@
         <v>848.95500000000004</v>
       </c>
       <c r="H25">
-        <v>532</v>
+        <v>472.89833329999999</v>
       </c>
       <c r="I25">
         <f t="shared" si="7"/>
@@ -11350,7 +11350,7 @@
         <v>851.31</v>
       </c>
       <c r="H26">
-        <v>532</v>
+        <v>463.21199999999999</v>
       </c>
       <c r="I26">
         <f t="shared" si="7"/>
@@ -11423,7 +11423,7 @@
         <v>849.44500000000005</v>
       </c>
       <c r="H27">
-        <v>532</v>
+        <v>432.53280000000001</v>
       </c>
       <c r="I27">
         <f t="shared" si="7"/>
@@ -11499,7 +11499,7 @@
         <v>849.14499999999998</v>
       </c>
       <c r="H28">
-        <v>520</v>
+        <v>410.94400000000002</v>
       </c>
       <c r="I28">
         <f t="shared" si="7"/>
@@ -11575,7 +11575,7 @@
         <v>839.24437499999999</v>
       </c>
       <c r="H29">
-        <v>510</v>
+        <v>400.03859999999997</v>
       </c>
       <c r="I29">
         <f t="shared" si="7"/>
@@ -11651,7 +11651,7 @@
         <v>829.23500000000001</v>
       </c>
       <c r="H30">
-        <v>500</v>
+        <v>389.16559999999998</v>
       </c>
       <c r="I30">
         <f t="shared" si="7"/>
@@ -11709,7 +11709,7 @@
         <v>801.36775</v>
       </c>
       <c r="H31">
-        <v>490</v>
+        <v>383.15249999999997</v>
       </c>
       <c r="I31">
         <f t="shared" si="7"/>
@@ -11767,7 +11767,7 @@
         <v>773.91700000000003</v>
       </c>
       <c r="H32">
-        <v>480</v>
+        <v>377.16320000000002</v>
       </c>
       <c r="I32">
         <f t="shared" si="7"/>
@@ -11825,7 +11825,7 @@
         <v>752.61400000000003</v>
       </c>
       <c r="H33">
-        <v>470</v>
+        <v>362.01006669999998</v>
       </c>
       <c r="I33">
         <f t="shared" si="7"/>
@@ -11883,7 +11883,7 @@
         <v>731.46833330000004</v>
       </c>
       <c r="H34">
-        <v>460</v>
+        <v>346.84533329999999</v>
       </c>
       <c r="I34">
         <f t="shared" si="7"/>
@@ -11941,7 +11941,7 @@
         <v>710.48</v>
       </c>
       <c r="H35">
-        <v>450</v>
+        <v>331.66899999999998</v>
       </c>
       <c r="I35">
         <f t="shared" si="7"/>
@@ -11999,7 +11999,7 @@
         <v>710.35866669999996</v>
       </c>
       <c r="H36">
-        <v>450</v>
+        <v>314.73022220000001</v>
       </c>
       <c r="I36">
         <f t="shared" si="7"/>
@@ -12057,7 +12057,7 @@
         <v>710.23733330000005</v>
       </c>
       <c r="H37">
-        <v>450</v>
+        <v>297.78388890000002</v>
       </c>
       <c r="I37">
         <f t="shared" si="7"/>
@@ -12115,7 +12115,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H38">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I38">
         <f t="shared" si="7"/>
@@ -12173,7 +12173,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H39">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I39">
         <f t="shared" si="7"/>
@@ -12231,7 +12231,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H40">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I40">
         <f t="shared" si="7"/>
@@ -12289,7 +12289,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H41">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I41">
         <f t="shared" si="7"/>
@@ -12347,7 +12347,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H42">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I42">
         <f t="shared" si="7"/>
@@ -12405,7 +12405,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H43">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I43">
         <f t="shared" si="7"/>
@@ -12463,7 +12463,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H44">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I44">
         <f t="shared" si="7"/>
@@ -12521,7 +12521,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H45">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I45">
         <f t="shared" si="7"/>
@@ -12579,7 +12579,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H46">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I46">
         <f t="shared" si="7"/>
@@ -12637,7 +12637,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H47">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I47">
         <f t="shared" si="7"/>
@@ -12695,7 +12695,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H48">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I48">
         <f t="shared" si="7"/>
@@ -12753,7 +12753,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H49">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I49">
         <f t="shared" si="7"/>
@@ -12811,7 +12811,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H50">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I50">
         <f t="shared" si="7"/>
@@ -12869,7 +12869,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H51">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I51">
         <f t="shared" si="7"/>
@@ -12927,7 +12927,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H52">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I52">
         <f t="shared" si="7"/>
@@ -12985,7 +12985,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H53">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I53">
         <f t="shared" si="7"/>
@@ -13043,7 +13043,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H54">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I54">
         <f t="shared" si="7"/>
@@ -13101,7 +13101,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H55">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I55">
         <f t="shared" si="7"/>
@@ -13159,7 +13159,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H56">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I56">
         <f t="shared" si="7"/>
@@ -13217,7 +13217,7 @@
         <v>710.11599999999999</v>
       </c>
       <c r="H57">
-        <v>450</v>
+        <v>280.83</v>
       </c>
       <c r="I57">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
working on energy analysis
and understanding inputs related to debugging
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/MaterialCompositionAnnual-Graph.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/MaterialCompositionAnnual-Graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642D5989-C3E8-426A-B852-E0EDE7F726C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D76C35-8795-4929-905E-319595C46042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6405" windowWidth="29040" windowHeight="15840" xr2:uid="{0FB8D6CD-8546-4236-B63D-A974CB21DD58}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0FB8D6CD-8546-4236-B63D-A974CB21DD58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>year</t>
   </si>
@@ -150,6 +150,30 @@
   </si>
   <si>
     <t xml:space="preserve">QUICK ENCAPSULANT </t>
+  </si>
+  <si>
+    <t>hex</t>
+  </si>
+  <si>
+    <t>#00bfbf</t>
+  </si>
+  <si>
+    <t>#ff7f0e</t>
+  </si>
+  <si>
+    <t>#1f77be</t>
+  </si>
+  <si>
+    <t>#2ca02c</t>
+  </si>
+  <si>
+    <t>#d62728</t>
+  </si>
+  <si>
+    <t>#9467BD</t>
+  </si>
+  <si>
+    <t>#8C564B</t>
   </si>
 </sst>
 </file>
@@ -3733,15 +3757,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>117474</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>111124</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>460374</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>115570</xdr:rowOff>
+      <xdr:colOff>454024</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>172720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4070,8 +4094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B855FEC6-71A0-4178-BC01-33F7B8382BFB}">
   <dimension ref="A1:AC57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:R28"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12:AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4952,6 +4976,30 @@
       <c r="R12" s="1">
         <f t="shared" si="9"/>
         <v>2.0651598432916138</v>
+      </c>
+      <c r="T12" t="s">
+        <v>33</v>
+      </c>
+      <c r="U12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V12" t="s">
+        <v>35</v>
+      </c>
+      <c r="W12" t="s">
+        <v>36</v>
+      </c>
+      <c r="X12" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
updating energy by component graph by making new journal in tutorials
plots annual stacked bar chart of energy demands by material and module, assuming no circularity.
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/MaterialCompositionAnnual-Graph.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/MaterialCompositionAnnual-Graph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB716AF-0462-43A3-B369-B41D6522E41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F44250-0108-4624-B988-301E3E994DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="28035" yWindow="8070" windowWidth="9600" windowHeight="4395" xr2:uid="{0FB8D6CD-8546-4236-B63D-A974CB21DD58}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0FB8D6CD-8546-4236-B63D-A974CB21DD58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3757,15 +3757,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>174624</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>34924</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>517524</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>77470</xdr:rowOff>
+      <xdr:colOff>377824</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4094,8 +4094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B855FEC6-71A0-4178-BC01-33F7B8382BFB}">
   <dimension ref="A1:AC57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29:P29"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
graphing tweak and reruning PVRW 2023
so that I have it in the temp folder on this, updating for Noreen and Susan data request.
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/MaterialCompositionAnnual-Graph.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/MaterialCompositionAnnual-Graph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBF1096-38DF-491C-A1A8-9CD63F8B4E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736F78A9-08A9-46ED-B96B-ED31A41D9E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0FB8D6CD-8546-4236-B63D-A974CB21DD58}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{0FB8D6CD-8546-4236-B63D-A974CB21DD58}"/>
   </bookViews>
   <sheets>
     <sheet name="Silicon" sheetId="1" r:id="rId1"/>
@@ -188,7 +188,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -347,13 +347,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -15891,7 +15891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FCC222-30DE-4579-B7D5-14187B1877AA}">
   <dimension ref="A1:AA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="AB47" sqref="AB47"/>
     </sheetView>
   </sheetViews>
@@ -15980,11 +15980,11 @@
       <c r="F2">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H2">
-        <f>SUM(B2:G2)</f>
+        <f t="shared" ref="H2:H33" si="0">SUM(B2:G2)</f>
         <v>16462.2</v>
       </c>
       <c r="I2">
@@ -15992,27 +15992,27 @@
         <v>16.462199999999999</v>
       </c>
       <c r="K2" s="1">
-        <f>B2/$H2*100</f>
+        <f t="shared" ref="K2:K33" si="1">B2/$H2*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L2" s="1">
-        <f>C2/$H2*100</f>
+        <f t="shared" ref="L2:L33" si="2">C2/$H2*100</f>
         <v>0</v>
       </c>
       <c r="M2" s="1">
-        <f>D2/$H2*100</f>
+        <f t="shared" ref="M2:M33" si="3">D2/$H2*100</f>
         <v>0.34351423260560554</v>
       </c>
       <c r="N2" s="1">
-        <f>E2/$H2*100</f>
+        <f t="shared" ref="N2:N33" si="4">E2/$H2*100</f>
         <v>2.3575220808883381</v>
       </c>
       <c r="O2" s="1">
-        <f t="shared" ref="O2:P17" si="0">F2/$H2*100</f>
+        <f t="shared" ref="O2:P17" si="5">F2/$H2*100</f>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P2" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>5.6677250671234712E-2</v>
       </c>
       <c r="W2" t="s">
@@ -16044,39 +16044,39 @@
       <c r="F3">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H3">
-        <f>SUM(B3:G3)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I57" si="1">H3/1000</f>
+        <f t="shared" ref="I3:I57" si="6">H3/1000</f>
         <v>16.462199999999999</v>
       </c>
       <c r="K3" s="1">
-        <f>B3/$H3*100</f>
+        <f t="shared" si="1"/>
         <v>97.192355821214662</v>
       </c>
       <c r="L3" s="1">
-        <f>C3/$H3*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M3" s="1">
-        <f>D3/$H3*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N3" s="1">
-        <f>E3/$H3*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P3" s="1">
-        <f>G3/$H3*100</f>
+        <f t="shared" ref="P3:P34" si="7">G3/$H3*100</f>
         <v>5.6677250671234712E-2</v>
       </c>
       <c r="W3" t="s">
@@ -16116,39 +16116,39 @@
       <c r="F4">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H4">
-        <f>SUM(B4:G4)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I4">
+        <f t="shared" si="6"/>
+        <v>16.462199999999999</v>
+      </c>
+      <c r="K4" s="1">
         <f t="shared" si="1"/>
-        <v>16.462199999999999</v>
-      </c>
-      <c r="K4" s="1">
-        <f>B4/$H4*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L4" s="1">
-        <f>C4/$H4*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M4" s="1">
-        <f>D4/$H4*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N4" s="1">
-        <f>E4/$H4*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P4" s="1">
-        <f>G4/$H4*100</f>
+        <f t="shared" si="7"/>
         <v>5.6677250671234712E-2</v>
       </c>
       <c r="W4" t="s">
@@ -16180,39 +16180,39 @@
       <c r="F5">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H5">
-        <f>SUM(B5:G5)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I5">
+        <f t="shared" si="6"/>
+        <v>16.462199999999999</v>
+      </c>
+      <c r="K5" s="1">
         <f t="shared" si="1"/>
-        <v>16.462199999999999</v>
-      </c>
-      <c r="K5" s="1">
-        <f>B5/$H5*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L5" s="1">
-        <f>C5/$H5*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M5" s="1">
-        <f>D5/$H5*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N5" s="1">
-        <f>E5/$H5*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P5" s="1">
-        <f>G5/$H5*100</f>
+        <f t="shared" si="7"/>
         <v>5.6677250671234712E-2</v>
       </c>
       <c r="X5">
@@ -16247,39 +16247,39 @@
       <c r="F6">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H6">
-        <f>SUM(B6:G6)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I6">
+        <f t="shared" si="6"/>
+        <v>16.462199999999999</v>
+      </c>
+      <c r="K6" s="1">
         <f t="shared" si="1"/>
-        <v>16.462199999999999</v>
-      </c>
-      <c r="K6" s="1">
-        <f>B6/$H6*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L6" s="1">
-        <f>C6/$H6*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M6" s="1">
-        <f>D6/$H6*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N6" s="1">
-        <f>E6/$H6*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P6" s="1">
-        <f>G6/$H6*100</f>
+        <f t="shared" si="7"/>
         <v>5.6677250671234712E-2</v>
       </c>
       <c r="W6" t="s">
@@ -16312,39 +16312,39 @@
       <c r="F7">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H7">
-        <f>SUM(B7:G7)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I7">
+        <f t="shared" si="6"/>
+        <v>16.462199999999999</v>
+      </c>
+      <c r="K7" s="1">
         <f t="shared" si="1"/>
-        <v>16.462199999999999</v>
-      </c>
-      <c r="K7" s="1">
-        <f>B7/$H7*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L7" s="1">
-        <f>C7/$H7*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M7" s="1">
-        <f>D7/$H7*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N7" s="1">
-        <f>E7/$H7*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P7" s="1">
-        <f>G7/$H7*100</f>
+        <f t="shared" si="7"/>
         <v>5.6677250671234712E-2</v>
       </c>
     </row>
@@ -16367,39 +16367,39 @@
       <c r="F8">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H8">
-        <f>SUM(B8:G8)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I8">
+        <f t="shared" si="6"/>
+        <v>16.462199999999999</v>
+      </c>
+      <c r="K8" s="1">
         <f t="shared" si="1"/>
-        <v>16.462199999999999</v>
-      </c>
-      <c r="K8" s="1">
-        <f>B8/$H8*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L8" s="1">
-        <f>C8/$H8*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M8" s="1">
-        <f>D8/$H8*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N8" s="1">
-        <f>E8/$H8*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P8" s="1">
-        <f>G8/$H8*100</f>
+        <f t="shared" si="7"/>
         <v>5.6677250671234712E-2</v>
       </c>
       <c r="S8" t="s">
@@ -16443,39 +16443,39 @@
       <c r="F9">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H9">
-        <f>SUM(B9:G9)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I9">
+        <f t="shared" si="6"/>
+        <v>16.462199999999999</v>
+      </c>
+      <c r="K9" s="1">
         <f t="shared" si="1"/>
-        <v>16.462199999999999</v>
-      </c>
-      <c r="K9" s="1">
-        <f>B9/$H9*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L9" s="1">
-        <f>C9/$H9*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M9" s="1">
-        <f>D9/$H9*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N9" s="1">
-        <f>E9/$H9*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P9" s="1">
-        <f>G9/$H9*100</f>
+        <f t="shared" si="7"/>
         <v>5.6677250671234712E-2</v>
       </c>
       <c r="R9" t="s">
@@ -16516,39 +16516,39 @@
       <c r="F10">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H10">
-        <f>SUM(B10:G10)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I10">
+        <f t="shared" si="6"/>
+        <v>16.462199999999999</v>
+      </c>
+      <c r="K10" s="1">
         <f t="shared" si="1"/>
-        <v>16.462199999999999</v>
-      </c>
-      <c r="K10" s="1">
-        <f>B10/$H10*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L10" s="1">
-        <f>C10/$H10*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M10" s="1">
-        <f>D10/$H10*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N10" s="1">
-        <f>E10/$H10*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P10" s="1">
-        <f>G10/$H10*100</f>
+        <f t="shared" si="7"/>
         <v>5.6677250671234712E-2</v>
       </c>
       <c r="R10" t="s">
@@ -16589,39 +16589,39 @@
       <c r="F11">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H11">
-        <f>SUM(B11:G11)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I11">
+        <f t="shared" si="6"/>
+        <v>16.462199999999999</v>
+      </c>
+      <c r="K11" s="1">
         <f t="shared" si="1"/>
-        <v>16.462199999999999</v>
-      </c>
-      <c r="K11" s="1">
-        <f>B11/$H11*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L11" s="1">
-        <f>C11/$H11*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M11" s="1">
-        <f>D11/$H11*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N11" s="1">
-        <f>E11/$H11*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P11" s="1">
-        <f>G11/$H11*100</f>
+        <f t="shared" si="7"/>
         <v>5.6677250671234712E-2</v>
       </c>
       <c r="R11" t="s">
@@ -16662,39 +16662,39 @@
       <c r="F12">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H12">
-        <f>SUM(B12:G12)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I12">
+        <f t="shared" si="6"/>
+        <v>16.462199999999999</v>
+      </c>
+      <c r="K12" s="1">
         <f t="shared" si="1"/>
-        <v>16.462199999999999</v>
-      </c>
-      <c r="K12" s="1">
-        <f>B12/$H12*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L12" s="1">
-        <f>C12/$H12*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M12" s="1">
-        <f>D12/$H12*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N12" s="1">
-        <f>E12/$H12*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P12" s="1">
-        <f>G12/$H12*100</f>
+        <f t="shared" si="7"/>
         <v>5.6677250671234712E-2</v>
       </c>
       <c r="R12" t="s">
@@ -16741,39 +16741,39 @@
       <c r="F13">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H13">
-        <f>SUM(B13:G13)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I13">
+        <f t="shared" si="6"/>
+        <v>16.462199999999999</v>
+      </c>
+      <c r="K13" s="1">
         <f t="shared" si="1"/>
-        <v>16.462199999999999</v>
-      </c>
-      <c r="K13" s="1">
-        <f>B13/$H13*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L13" s="1">
-        <f>C13/$H13*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M13" s="1">
-        <f>D13/$H13*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N13" s="1">
-        <f>E13/$H13*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P13" s="1">
-        <f>G13/$H13*100</f>
+        <f t="shared" si="7"/>
         <v>5.6677250671234712E-2</v>
       </c>
     </row>
@@ -16796,39 +16796,39 @@
       <c r="F14">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H14">
-        <f>SUM(B14:G14)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I14">
+        <f t="shared" si="6"/>
+        <v>16.462199999999999</v>
+      </c>
+      <c r="K14" s="1">
         <f t="shared" si="1"/>
-        <v>16.462199999999999</v>
-      </c>
-      <c r="K14" s="1">
-        <f>B14/$H14*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L14" s="1">
-        <f>C14/$H14*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M14" s="1">
-        <f>D14/$H14*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N14" s="1">
-        <f>E14/$H14*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P14" s="1">
-        <f>G14/$H14*100</f>
+        <f t="shared" si="7"/>
         <v>5.6677250671234712E-2</v>
       </c>
     </row>
@@ -16851,39 +16851,39 @@
       <c r="F15">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H15">
-        <f>SUM(B15:G15)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I15">
+        <f t="shared" si="6"/>
+        <v>16.462199999999999</v>
+      </c>
+      <c r="K15" s="1">
         <f t="shared" si="1"/>
-        <v>16.462199999999999</v>
-      </c>
-      <c r="K15" s="1">
-        <f>B15/$H15*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L15" s="1">
-        <f>C15/$H15*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M15" s="1">
-        <f>D15/$H15*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N15" s="1">
-        <f>E15/$H15*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P15" s="1">
-        <f>G15/$H15*100</f>
+        <f t="shared" si="7"/>
         <v>5.6677250671234712E-2</v>
       </c>
     </row>
@@ -16906,39 +16906,39 @@
       <c r="F16">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H16">
-        <f>SUM(B16:G16)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I16">
+        <f t="shared" si="6"/>
+        <v>16.462199999999999</v>
+      </c>
+      <c r="K16" s="1">
         <f t="shared" si="1"/>
-        <v>16.462199999999999</v>
-      </c>
-      <c r="K16" s="1">
-        <f>B16/$H16*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L16" s="1">
-        <f>C16/$H16*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M16" s="1">
-        <f>D16/$H16*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N16" s="1">
-        <f>E16/$H16*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P16" s="1">
-        <f>G16/$H16*100</f>
+        <f t="shared" si="7"/>
         <v>5.6677250671234712E-2</v>
       </c>
     </row>
@@ -16961,39 +16961,39 @@
       <c r="F17">
         <v>8.2196776400000005</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="16">
         <v>9.3303223600000003</v>
       </c>
       <c r="H17">
-        <f>SUM(B17:G17)</f>
+        <f t="shared" si="0"/>
         <v>16462.2</v>
       </c>
       <c r="I17">
+        <f t="shared" si="6"/>
+        <v>16.462199999999999</v>
+      </c>
+      <c r="K17" s="1">
         <f t="shared" si="1"/>
-        <v>16.462199999999999</v>
-      </c>
-      <c r="K17" s="1">
-        <f>B17/$H17*100</f>
         <v>97.192355821214662</v>
       </c>
       <c r="L17" s="1">
-        <f>C17/$H17*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M17" s="1">
-        <f>D17/$H17*100</f>
+        <f t="shared" si="3"/>
         <v>0.34351423260560554</v>
       </c>
       <c r="N17" s="1">
-        <f>E17/$H17*100</f>
+        <f t="shared" si="4"/>
         <v>2.3575220808883381</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.9930614620160123E-2</v>
       </c>
       <c r="P17" s="1">
-        <f>G17/$H17*100</f>
+        <f t="shared" si="7"/>
         <v>5.6677250671234712E-2</v>
       </c>
     </row>
@@ -17016,39 +17016,39 @@
       <c r="F18">
         <v>6.0277636030000004</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H18">
-        <f>SUM(B18:G18)</f>
+        <f t="shared" si="0"/>
         <v>16457.519999999997</v>
       </c>
       <c r="I18">
+        <f t="shared" si="6"/>
+        <v>16.457519999999995</v>
+      </c>
+      <c r="K18" s="1">
         <f t="shared" si="1"/>
-        <v>16.457519999999995</v>
-      </c>
-      <c r="K18" s="1">
-        <f>B18/$H18*100</f>
         <v>97.219994264020357</v>
       </c>
       <c r="L18" s="1">
-        <f>C18/$H18*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M18" s="1">
-        <f>D18/$H18*100</f>
+        <f t="shared" si="3"/>
         <v>0.34361191722689693</v>
       </c>
       <c r="N18" s="1">
-        <f>E18/$H18*100</f>
+        <f t="shared" si="4"/>
         <v>2.3581924858666441</v>
       </c>
       <c r="O18" s="1">
-        <f t="shared" ref="O18:O57" si="2">F18/$H18*100</f>
+        <f t="shared" ref="O18:O57" si="8">F18/$H18*100</f>
         <v>3.6626196431783171E-2</v>
       </c>
       <c r="P18" s="1">
-        <f>G18/$H18*100</f>
+        <f t="shared" si="7"/>
         <v>4.1575136454338205E-2</v>
       </c>
     </row>
@@ -17071,39 +17071,39 @@
       <c r="F19">
         <v>6.0277636030000004</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H19">
-        <f>SUM(B19:G19)</f>
+        <f t="shared" si="0"/>
         <v>16457.519999999997</v>
       </c>
       <c r="I19">
+        <f t="shared" si="6"/>
+        <v>16.457519999999995</v>
+      </c>
+      <c r="K19" s="1">
         <f t="shared" si="1"/>
-        <v>16.457519999999995</v>
-      </c>
-      <c r="K19" s="1">
-        <f>B19/$H19*100</f>
         <v>97.219994264020357</v>
       </c>
       <c r="L19" s="1">
-        <f>C19/$H19*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M19" s="1">
-        <f>D19/$H19*100</f>
+        <f t="shared" si="3"/>
         <v>0.34361191722689693</v>
       </c>
       <c r="N19" s="1">
-        <f>E19/$H19*100</f>
+        <f t="shared" si="4"/>
         <v>2.3581924858666441</v>
       </c>
       <c r="O19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.6626196431783171E-2</v>
       </c>
       <c r="P19" s="1">
-        <f>G19/$H19*100</f>
+        <f t="shared" si="7"/>
         <v>4.1575136454338205E-2</v>
       </c>
     </row>
@@ -17126,39 +17126,39 @@
       <c r="F20">
         <v>6.0277636030000004</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H20">
-        <f>SUM(B20:G20)</f>
+        <f t="shared" si="0"/>
         <v>16457.519999999997</v>
       </c>
       <c r="I20">
+        <f t="shared" si="6"/>
+        <v>16.457519999999995</v>
+      </c>
+      <c r="K20" s="1">
         <f t="shared" si="1"/>
-        <v>16.457519999999995</v>
-      </c>
-      <c r="K20" s="1">
-        <f>B20/$H20*100</f>
         <v>97.219994264020357</v>
       </c>
       <c r="L20" s="1">
-        <f>C20/$H20*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M20" s="1">
-        <f>D20/$H20*100</f>
+        <f t="shared" si="3"/>
         <v>0.34361191722689693</v>
       </c>
       <c r="N20" s="1">
-        <f>E20/$H20*100</f>
+        <f t="shared" si="4"/>
         <v>2.3581924858666441</v>
       </c>
       <c r="O20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.6626196431783171E-2</v>
       </c>
       <c r="P20" s="1">
-        <f>G20/$H20*100</f>
+        <f t="shared" si="7"/>
         <v>4.1575136454338205E-2</v>
       </c>
     </row>
@@ -17181,39 +17181,39 @@
       <c r="F21">
         <v>6.0277636030000004</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H21">
-        <f>SUM(B21:G21)</f>
+        <f t="shared" si="0"/>
         <v>16405.019999999997</v>
       </c>
       <c r="I21">
+        <f t="shared" si="6"/>
+        <v>16.405019999999997</v>
+      </c>
+      <c r="K21" s="1">
         <f t="shared" si="1"/>
-        <v>16.405019999999997</v>
-      </c>
-      <c r="K21" s="1">
-        <f>B21/$H21*100</f>
         <v>97.211097578668017</v>
       </c>
       <c r="L21" s="1">
-        <f>C21/$H21*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M21" s="1">
-        <f>D21/$H21*100</f>
+        <f t="shared" si="3"/>
         <v>0.34471155780364793</v>
       </c>
       <c r="N21" s="1">
-        <f>E21/$H21*100</f>
+        <f t="shared" si="4"/>
         <v>2.3657392676144258</v>
       </c>
       <c r="O21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.6743409047962153E-2</v>
       </c>
       <c r="P21" s="1">
-        <f>G21/$H21*100</f>
+        <f t="shared" si="7"/>
         <v>4.1708186865971518E-2</v>
       </c>
     </row>
@@ -17236,39 +17236,39 @@
       <c r="F22">
         <v>6.0277636030000004</v>
       </c>
-      <c r="G22" s="18">
+      <c r="G22" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H22">
-        <f>SUM(B22:G22)</f>
+        <f t="shared" si="0"/>
         <v>16352.52</v>
       </c>
       <c r="I22">
+        <f t="shared" si="6"/>
+        <v>16.352520000000002</v>
+      </c>
+      <c r="K22" s="1">
         <f t="shared" si="1"/>
-        <v>16.352520000000002</v>
-      </c>
-      <c r="K22" s="1">
-        <f>B22/$H22*100</f>
         <v>97.2021437674438</v>
       </c>
       <c r="L22" s="1">
-        <f>C22/$H22*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M22" s="1">
-        <f>D22/$H22*100</f>
+        <f t="shared" si="3"/>
         <v>0.34581825920408599</v>
       </c>
       <c r="N22" s="1">
-        <f>E22/$H22*100</f>
+        <f t="shared" si="4"/>
         <v>2.3733345074642931</v>
       </c>
       <c r="O22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.6861374289711923E-2</v>
       </c>
       <c r="P22" s="1">
-        <f>G22/$H22*100</f>
+        <f t="shared" si="7"/>
         <v>4.1842091598114542E-2</v>
       </c>
     </row>
@@ -17291,39 +17291,39 @@
       <c r="F23">
         <v>6.0277636030000004</v>
       </c>
-      <c r="G23" s="18">
+      <c r="G23" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H23">
-        <f>SUM(B23:G23)</f>
+        <f t="shared" si="0"/>
         <v>16300.02</v>
       </c>
       <c r="I23">
+        <f t="shared" si="6"/>
+        <v>16.30002</v>
+      </c>
+      <c r="K23" s="1">
         <f t="shared" si="1"/>
-        <v>16.30002</v>
-      </c>
-      <c r="K23" s="1">
-        <f>B23/$H23*100</f>
         <v>97.193132278365297</v>
       </c>
       <c r="L23" s="1">
-        <f>C23/$H23*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M23" s="1">
-        <f>D23/$H23*100</f>
+        <f t="shared" si="3"/>
         <v>0.34693208965387767</v>
       </c>
       <c r="N23" s="1">
-        <f>E23/$H23*100</f>
+        <f t="shared" si="4"/>
         <v>2.380978673645799</v>
       </c>
       <c r="O23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.6980099429325855E-2</v>
       </c>
       <c r="P23" s="1">
-        <f>G23/$H23*100</f>
+        <f t="shared" si="7"/>
         <v>4.1976858905694588E-2</v>
       </c>
     </row>
@@ -17346,39 +17346,39 @@
       <c r="F24">
         <v>6.0277636030000004</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H24">
-        <f>SUM(B24:G24)</f>
+        <f t="shared" si="0"/>
         <v>16247.52</v>
       </c>
       <c r="I24">
+        <f t="shared" si="6"/>
+        <v>16.247520000000002</v>
+      </c>
+      <c r="K24" s="1">
         <f t="shared" si="1"/>
-        <v>16.247520000000002</v>
-      </c>
-      <c r="K24" s="1">
-        <f>B24/$H24*100</f>
         <v>97.18406255231568</v>
       </c>
       <c r="L24" s="1">
-        <f>C24/$H24*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M24" s="1">
-        <f>D24/$H24*100</f>
+        <f t="shared" si="3"/>
         <v>0.34805311826050989</v>
       </c>
       <c r="N24" s="1">
-        <f>E24/$H24*100</f>
+        <f t="shared" si="4"/>
         <v>2.3886722404403873</v>
       </c>
       <c r="O24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.7099591833092069E-2</v>
       </c>
       <c r="P24" s="1">
-        <f>G24/$H24*100</f>
+        <f t="shared" si="7"/>
         <v>4.2112497150334327E-2</v>
       </c>
     </row>
@@ -17401,39 +17401,39 @@
       <c r="F25">
         <v>6.0277636030000004</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G25" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H25">
-        <f>SUM(B25:G25)</f>
+        <f t="shared" si="0"/>
         <v>16330.052683100001</v>
       </c>
       <c r="I25">
+        <f t="shared" si="6"/>
+        <v>16.3300526831</v>
+      </c>
+      <c r="K25" s="1">
         <f t="shared" si="1"/>
-        <v>16.3300526831</v>
-      </c>
-      <c r="K25" s="1">
-        <f>B25/$H25*100</f>
         <v>96.478561984707355</v>
       </c>
       <c r="L25" s="1">
-        <f>C25/$H25*100</f>
+        <f t="shared" si="2"/>
         <v>0.71973241838732571</v>
       </c>
       <c r="M25" s="1">
-        <f>D25/$H25*100</f>
+        <f t="shared" si="3"/>
         <v>0.34629404507998734</v>
       </c>
       <c r="N25" s="1">
-        <f>E25/$H25*100</f>
+        <f t="shared" si="4"/>
         <v>2.3765998036347145</v>
       </c>
       <c r="O25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.6912089140031634E-2</v>
       </c>
       <c r="P25" s="1">
-        <f>G25/$H25*100</f>
+        <f t="shared" si="7"/>
         <v>4.1899659050586173E-2</v>
       </c>
     </row>
@@ -17456,39 +17456,39 @@
       <c r="F26">
         <v>6.0277636030000004</v>
       </c>
-      <c r="G26" s="18">
+      <c r="G26" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H26">
-        <f>SUM(B26:G26)</f>
+        <f t="shared" si="0"/>
         <v>16309.6002826</v>
       </c>
       <c r="I26">
+        <f t="shared" si="6"/>
+        <v>16.309600282600002</v>
+      </c>
+      <c r="K26" s="1">
         <f t="shared" si="1"/>
-        <v>16.309600282600002</v>
-      </c>
-      <c r="K26" s="1">
-        <f>B26/$H26*100</f>
         <v>95.955754456449199</v>
       </c>
       <c r="L26" s="1">
-        <f>C26/$H26*100</f>
+        <f t="shared" si="2"/>
         <v>1.2390265800418825</v>
       </c>
       <c r="M26" s="1">
-        <f>D26/$H26*100</f>
+        <f t="shared" si="3"/>
         <v>0.34672830124678605</v>
       </c>
       <c r="N26" s="1">
-        <f>E26/$H26*100</f>
+        <f t="shared" si="4"/>
         <v>2.3795800833576952</v>
       </c>
       <c r="O26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.6958377265877924E-2</v>
       </c>
       <c r="P26" s="1">
-        <f>G26/$H26*100</f>
+        <f t="shared" si="7"/>
         <v>4.1952201638563037E-2</v>
       </c>
     </row>
@@ -17511,39 +17511,39 @@
       <c r="F27">
         <v>6.0277636030000004</v>
       </c>
-      <c r="G27" s="18">
+      <c r="G27" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H27">
-        <f>SUM(B27:G27)</f>
+        <f t="shared" si="0"/>
         <v>16338.2739683</v>
       </c>
       <c r="I27">
+        <f t="shared" si="6"/>
+        <v>16.338273968300001</v>
+      </c>
+      <c r="K27" s="1">
         <f t="shared" si="1"/>
-        <v>16.338273968300001</v>
-      </c>
-      <c r="K27" s="1">
-        <f>B27/$H27*100</f>
         <v>94.716247444650818</v>
       </c>
       <c r="L27" s="1">
-        <f>C27/$H27*100</f>
+        <f t="shared" si="2"/>
         <v>2.4834567536770149</v>
       </c>
       <c r="M27" s="1">
-        <f>D27/$H27*100</f>
+        <f t="shared" si="3"/>
         <v>0.34611979276219734</v>
       </c>
       <c r="N27" s="1">
-        <f>E27/$H27*100</f>
+        <f t="shared" si="4"/>
         <v>2.3754039181433919</v>
       </c>
       <c r="O27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.6893515280103914E-2</v>
       </c>
       <c r="P27" s="1">
-        <f>G27/$H27*100</f>
+        <f t="shared" si="7"/>
         <v>4.1878575486465147E-2</v>
       </c>
     </row>
@@ -17566,39 +17566,39 @@
       <c r="F28">
         <v>6.0277636030000004</v>
       </c>
-      <c r="G28" s="18">
+      <c r="G28" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H28">
-        <f>SUM(B28:G28)</f>
+        <f t="shared" si="0"/>
         <v>16184.027936500001</v>
       </c>
       <c r="I28">
+        <f t="shared" si="6"/>
+        <v>16.184027936500001</v>
+      </c>
+      <c r="K28" s="1">
         <f t="shared" si="1"/>
-        <v>16.184027936500001</v>
-      </c>
-      <c r="K28" s="1">
-        <f>B28/$H28*100</f>
         <v>92.158763309855956</v>
       </c>
       <c r="L28" s="1">
-        <f>C28/$H28*100</f>
+        <f t="shared" si="2"/>
         <v>5.0142519506519019</v>
       </c>
       <c r="M28" s="1">
-        <f>D28/$H28*100</f>
+        <f t="shared" si="3"/>
         <v>0.34941857627706024</v>
       </c>
       <c r="N28" s="1">
-        <f>E28/$H28*100</f>
+        <f t="shared" si="4"/>
         <v>2.3980433148209923</v>
       </c>
       <c r="O28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.7245138396020214E-2</v>
       </c>
       <c r="P28" s="1">
-        <f>G28/$H28*100</f>
+        <f t="shared" si="7"/>
         <v>4.2277709998069367E-2</v>
       </c>
     </row>
@@ -17621,39 +17621,39 @@
       <c r="F29">
         <v>6.0277636030000004</v>
       </c>
-      <c r="G29" s="18">
+      <c r="G29" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H29">
-        <f>SUM(B29:G29)</f>
+        <f t="shared" si="0"/>
         <v>16079.027936500001</v>
       </c>
       <c r="I29">
+        <f t="shared" si="6"/>
+        <v>16.079027936500001</v>
+      </c>
+      <c r="K29" s="1">
         <f t="shared" si="1"/>
-        <v>16.079027936500001</v>
-      </c>
-      <c r="K29" s="1">
-        <f>B29/$H29*100</f>
         <v>92.107558109161189</v>
       </c>
       <c r="L29" s="1">
-        <f>C29/$H29*100</f>
+        <f t="shared" si="2"/>
         <v>5.0469962469425553</v>
       </c>
       <c r="M29" s="1">
-        <f>D29/$H29*100</f>
+        <f t="shared" si="3"/>
         <v>0.35170036536617594</v>
       </c>
       <c r="N29" s="1">
-        <f>E29/$H29*100</f>
+        <f t="shared" si="4"/>
         <v>2.4137031264122526</v>
       </c>
       <c r="O29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.7488358293829127E-2</v>
       </c>
       <c r="P29" s="1">
-        <f>G29/$H29*100</f>
+        <f t="shared" si="7"/>
         <v>4.2553793823990223E-2</v>
       </c>
     </row>
@@ -17676,39 +17676,39 @@
       <c r="F30">
         <v>6.0277636030000004</v>
       </c>
-      <c r="G30" s="18">
+      <c r="G30" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H30">
-        <f>SUM(B30:G30)</f>
+        <f t="shared" si="0"/>
         <v>15904.027936500001</v>
       </c>
       <c r="I30">
+        <f t="shared" si="6"/>
+        <v>15.9040279365</v>
+      </c>
+      <c r="K30" s="1">
         <f t="shared" si="1"/>
-        <v>15.9040279365</v>
-      </c>
-      <c r="K30" s="1">
-        <f>B30/$H30*100</f>
         <v>92.020713610622124</v>
       </c>
       <c r="L30" s="1">
-        <f>C30/$H30*100</f>
+        <f t="shared" si="2"/>
         <v>5.1025308792219626</v>
       </c>
       <c r="M30" s="1">
-        <f>D30/$H30*100</f>
+        <f t="shared" si="3"/>
         <v>0.35557030096895664</v>
       </c>
       <c r="N30" s="1">
-        <f>E30/$H30*100</f>
+        <f t="shared" si="4"/>
         <v>2.4402623131043697</v>
       </c>
       <c r="O30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.790086151173179E-2</v>
       </c>
       <c r="P30" s="1">
-        <f>G30/$H30*100</f>
+        <f t="shared" si="7"/>
         <v>4.3022034570858347E-2</v>
       </c>
     </row>
@@ -17731,39 +17731,39 @@
       <c r="F31">
         <v>6.0277636030000004</v>
       </c>
-      <c r="G31" s="18">
+      <c r="G31" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H31">
-        <f>SUM(B31:G31)</f>
+        <f t="shared" si="0"/>
         <v>16134.781905</v>
       </c>
       <c r="I31">
+        <f t="shared" si="6"/>
+        <v>16.134781905000001</v>
+      </c>
+      <c r="K31" s="1">
         <f t="shared" si="1"/>
-        <v>16.134781905000001</v>
-      </c>
-      <c r="K31" s="1">
-        <f>B31/$H31*100</f>
         <v>89.620052413097682</v>
       </c>
       <c r="L31" s="1">
-        <f>C31/$H31*100</f>
+        <f t="shared" si="2"/>
         <v>7.5443344209244216</v>
       </c>
       <c r="M31" s="1">
-        <f>D31/$H31*100</f>
+        <f t="shared" si="3"/>
         <v>0.35048505974831767</v>
       </c>
       <c r="N31" s="1">
-        <f>E31/$H31*100</f>
+        <f t="shared" si="4"/>
         <v>2.4053625409075527</v>
       </c>
       <c r="O31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.7358816738217331E-2</v>
       </c>
       <c r="P31" s="1">
-        <f>G31/$H31*100</f>
+        <f t="shared" si="7"/>
         <v>4.2406748583813596E-2</v>
       </c>
     </row>
@@ -17786,39 +17786,39 @@
       <c r="F32">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G32" s="18">
+      <c r="G32" s="16">
         <v>6.8422363969999997</v>
       </c>
       <c r="H32">
-        <f>SUM(B32:G32)</f>
+        <f t="shared" si="0"/>
         <v>16382.487894490001</v>
       </c>
       <c r="I32">
+        <f t="shared" si="6"/>
+        <v>16.382487894490001</v>
+      </c>
+      <c r="K32" s="1">
         <f t="shared" si="1"/>
-        <v>16.382487894490001</v>
-      </c>
-      <c r="K32" s="1">
-        <f>B32/$H32*100</f>
         <v>87.303589614190571</v>
       </c>
       <c r="L32" s="1">
-        <f>C32/$H32*100</f>
+        <f t="shared" si="2"/>
         <v>9.9070170748966451</v>
       </c>
       <c r="M32" s="1">
-        <f>D32/$H32*100</f>
+        <f t="shared" si="3"/>
         <v>0.34518566632983583</v>
       </c>
       <c r="N32" s="1">
-        <f>E32/$H32*100</f>
+        <f t="shared" si="4"/>
         <v>2.3689930522123657</v>
       </c>
       <c r="O32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.3449041002148655E-2</v>
       </c>
       <c r="P32" s="1">
-        <f>G32/$H32*100</f>
+        <f t="shared" si="7"/>
         <v>4.1765551368429708E-2</v>
       </c>
     </row>
@@ -17841,39 +17841,39 @@
       <c r="F33">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G33" s="18">
+      <c r="G33" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H33">
-        <f>SUM(B33:G33)</f>
+        <f t="shared" si="0"/>
         <v>16224.365873000001</v>
       </c>
       <c r="I33">
+        <f t="shared" si="6"/>
+        <v>16.224365873</v>
+      </c>
+      <c r="K33" s="1">
         <f t="shared" si="1"/>
-        <v>16.224365873</v>
-      </c>
-      <c r="K33" s="1">
-        <f>B33/$H33*100</f>
         <v>87.183684778334509</v>
       </c>
       <c r="L33" s="1">
-        <f>C33/$H33*100</f>
+        <f t="shared" si="2"/>
         <v>10.003570467434811</v>
       </c>
       <c r="M33" s="1">
-        <f>D33/$H33*100</f>
+        <f t="shared" si="3"/>
         <v>0.34854983204063744</v>
       </c>
       <c r="N33" s="1">
-        <f>E33/$H33*100</f>
+        <f t="shared" si="4"/>
         <v>2.3920811638368065</v>
       </c>
       <c r="O33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.3775034019167795E-2</v>
       </c>
       <c r="P33" s="1">
-        <f>G33/$H33*100</f>
+        <f t="shared" si="7"/>
         <v>3.8338724334067535E-2</v>
       </c>
     </row>
@@ -17896,39 +17896,39 @@
       <c r="F34">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G34" s="18">
+      <c r="G34" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H34">
-        <f>SUM(B34:G34)</f>
+        <f t="shared" ref="H34:H65" si="9">SUM(B34:G34)</f>
         <v>15736.945234999999</v>
       </c>
       <c r="I34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>15.736945234999999</v>
       </c>
       <c r="K34" s="1">
-        <f>B34/$H34*100</f>
+        <f t="shared" ref="K34:K57" si="10">B34/$H34*100</f>
         <v>89.365077656381644</v>
       </c>
       <c r="L34" s="1">
-        <f>C34/$H34*100</f>
+        <f t="shared" ref="L34:L57" si="11">C34/$H34*100</f>
         <v>7.7350584044273711</v>
       </c>
       <c r="M34" s="1">
-        <f>D34/$H34*100</f>
+        <f t="shared" ref="M34:M57" si="12">D34/$H34*100</f>
         <v>0.35934547115426879</v>
       </c>
       <c r="N34" s="1">
-        <f>E34/$H34*100</f>
+        <f t="shared" ref="N34:N57" si="13">E34/$H34*100</f>
         <v>2.4661711291772188</v>
       </c>
       <c r="O34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.4821148648421285E-2</v>
       </c>
       <c r="P34" s="1">
-        <f>G34/$H34*100</f>
+        <f t="shared" si="7"/>
         <v>3.9526190211082605E-2</v>
       </c>
     </row>
@@ -17951,39 +17951,39 @@
       <c r="F35">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G35" s="18">
+      <c r="G35" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H35">
-        <f>SUM(B35:G35)</f>
+        <f t="shared" si="9"/>
         <v>15249.524606500001</v>
       </c>
       <c r="I35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>15.249524606500001</v>
       </c>
       <c r="K35" s="1">
-        <f>B35/$H35*100</f>
+        <f t="shared" si="10"/>
         <v>91.685918287842327</v>
       </c>
       <c r="L35" s="1">
-        <f>C35/$H35*100</f>
+        <f t="shared" si="11"/>
         <v>5.3215294079010214</v>
       </c>
       <c r="M35" s="1">
-        <f>D35/$H35*100</f>
+        <f t="shared" si="12"/>
         <v>0.37083123218081149</v>
       </c>
       <c r="N35" s="1">
-        <f>E35/$H35*100</f>
+        <f t="shared" si="13"/>
         <v>2.5449973688660115</v>
       </c>
       <c r="O35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.5934137190508093E-2</v>
       </c>
       <c r="P35" s="1">
-        <f>G35/$H35*100</f>
+        <f t="shared" ref="P35:P57" si="14">G35/$H35*100</f>
         <v>4.0789566019314973E-2</v>
       </c>
     </row>
@@ -18006,39 +18006,39 @@
       <c r="F36">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G36" s="18">
+      <c r="G36" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H36">
-        <f>SUM(B36:G36)</f>
+        <f t="shared" si="9"/>
         <v>15167.857936500001</v>
       </c>
       <c r="I36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>15.167857936500001</v>
       </c>
       <c r="K36" s="1">
-        <f>B36/$H36*100</f>
+        <f t="shared" si="10"/>
         <v>91.641153669767561</v>
       </c>
       <c r="L36" s="1">
-        <f>C36/$H36*100</f>
+        <f t="shared" si="11"/>
         <v>5.3501815477001777</v>
       </c>
       <c r="M36" s="1">
-        <f>D36/$H36*100</f>
+        <f t="shared" si="12"/>
         <v>0.37282785899462989</v>
       </c>
       <c r="N36" s="1">
-        <f>E36/$H36*100</f>
+        <f t="shared" si="13"/>
         <v>2.558700125124949</v>
       </c>
       <c r="O36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.6127613509706079E-2</v>
       </c>
       <c r="P36" s="1">
-        <f>G36/$H36*100</f>
+        <f t="shared" si="14"/>
         <v>4.1009184902975962E-2</v>
       </c>
     </row>
@@ -18061,39 +18061,39 @@
       <c r="F37">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G37" s="18">
+      <c r="G37" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H37">
-        <f>SUM(B37:G37)</f>
+        <f t="shared" si="9"/>
         <v>15074.524606500001</v>
       </c>
       <c r="I37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>15.074524606500001</v>
       </c>
       <c r="K37" s="1">
-        <f>B37/$H37*100</f>
+        <f t="shared" si="10"/>
         <v>91.589400199371383</v>
       </c>
       <c r="L37" s="1">
-        <f>C37/$H37*100</f>
+        <f t="shared" si="11"/>
         <v>5.3833069876716708</v>
       </c>
       <c r="M37" s="1">
-        <f>D37/$H37*100</f>
+        <f t="shared" si="12"/>
         <v>0.3751362081137613</v>
       </c>
       <c r="N37" s="1">
-        <f>E37/$H37*100</f>
+        <f t="shared" si="13"/>
         <v>2.5745422169575733</v>
       </c>
       <c r="O37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.635129621691132E-2</v>
       </c>
       <c r="P37" s="1">
-        <f>G37/$H37*100</f>
+        <f t="shared" si="14"/>
         <v>4.126309166869447E-2</v>
       </c>
     </row>
@@ -18116,39 +18116,39 @@
       <c r="F38">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G38" s="18">
+      <c r="G38" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H38">
-        <f>SUM(B38:G38)</f>
+        <f t="shared" si="9"/>
         <v>14575.437298299999</v>
       </c>
       <c r="I38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.575437298299999</v>
       </c>
       <c r="K38" s="1">
-        <f>B38/$H38*100</f>
+        <f t="shared" si="10"/>
         <v>94.085227422984076</v>
       </c>
       <c r="L38" s="1">
-        <f>C38/$H38*100</f>
+        <f t="shared" si="11"/>
         <v>2.7838202037843827</v>
       </c>
       <c r="M38" s="1">
-        <f>D38/$H38*100</f>
+        <f t="shared" si="12"/>
         <v>0.38798149820585953</v>
       </c>
       <c r="N38" s="1">
-        <f>E38/$H38*100</f>
+        <f t="shared" si="13"/>
         <v>2.662698840914131</v>
       </c>
       <c r="O38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.7596025291393026E-2</v>
       </c>
       <c r="P38" s="1">
-        <f>G38/$H38*100</f>
+        <f t="shared" si="14"/>
         <v>4.2676008820164132E-2</v>
       </c>
     </row>
@@ -18171,39 +18171,39 @@
       <c r="F39">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G39" s="18">
+      <c r="G39" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H39">
-        <f>SUM(B39:G39)</f>
+        <f t="shared" si="9"/>
         <v>14278.4302826</v>
       </c>
       <c r="I39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.2784302826</v>
       </c>
       <c r="K39" s="1">
-        <f>B39/$H39*100</f>
+        <f t="shared" si="10"/>
         <v>95.388636778915554</v>
       </c>
       <c r="L39" s="1">
-        <f>C39/$H39*100</f>
+        <f t="shared" si="11"/>
         <v>1.4152836033121885</v>
       </c>
       <c r="M39" s="1">
-        <f>D39/$H39*100</f>
+        <f t="shared" si="12"/>
         <v>0.39605193904902158</v>
       </c>
       <c r="N39" s="1">
-        <f>E39/$H39*100</f>
+        <f t="shared" si="13"/>
         <v>2.7180858982303322</v>
       </c>
       <c r="O39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8378063866570708E-2</v>
       </c>
       <c r="P39" s="1">
-        <f>G39/$H39*100</f>
+        <f t="shared" si="14"/>
         <v>4.3563716626330323E-2</v>
       </c>
     </row>
@@ -18226,39 +18226,39 @@
       <c r="F40">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G40" s="18">
+      <c r="G40" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H40">
-        <f>SUM(B40:G40)</f>
+        <f t="shared" si="9"/>
         <v>14193.882683100001</v>
       </c>
       <c r="I40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.1938826831</v>
       </c>
       <c r="K40" s="1">
-        <f>B40/$H40*100</f>
+        <f t="shared" si="10"/>
         <v>95.956830869235688</v>
       </c>
       <c r="L40" s="1">
-        <f>C40/$H40*100</f>
+        <f t="shared" si="11"/>
         <v>0.82805167355610687</v>
       </c>
       <c r="M40" s="1">
-        <f>D40/$H40*100</f>
+        <f t="shared" si="12"/>
         <v>0.39841107089980016</v>
       </c>
       <c r="N40" s="1">
-        <f>E40/$H40*100</f>
+        <f t="shared" si="13"/>
         <v>2.7342765095705119</v>
       </c>
       <c r="O40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8606667501377381E-2</v>
       </c>
       <c r="P40" s="1">
-        <f>G40/$H40*100</f>
+        <f t="shared" si="14"/>
         <v>4.3823209236512305E-2</v>
       </c>
     </row>
@@ -18281,39 +18281,39 @@
       <c r="F41">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G41" s="18">
+      <c r="G41" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H41">
-        <f>SUM(B41:G41)</f>
+        <f t="shared" si="9"/>
         <v>14157.500793650001</v>
       </c>
       <c r="I41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.15750079365</v>
       </c>
       <c r="K41" s="1">
-        <f>B41/$H41*100</f>
+        <f t="shared" si="10"/>
         <v>96.203420353039405</v>
       </c>
       <c r="L41" s="1">
-        <f>C41/$H41*100</f>
+        <f t="shared" si="11"/>
         <v>0.57319999364858376</v>
       </c>
       <c r="M41" s="1">
-        <f>D41/$H41*100</f>
+        <f t="shared" si="12"/>
         <v>0.39943490609136401</v>
       </c>
       <c r="N41" s="1">
-        <f>E41/$H41*100</f>
+        <f t="shared" si="13"/>
         <v>2.7413030425120848</v>
       </c>
       <c r="O41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8705878762569611E-2</v>
       </c>
       <c r="P41" s="1">
-        <f>G41/$H41*100</f>
+        <f t="shared" si="14"/>
         <v>4.3935825945988466E-2</v>
       </c>
     </row>
@@ -18336,39 +18336,39 @@
       <c r="F42">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G42" s="18">
+      <c r="G42" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H42">
-        <f>SUM(B42:G42)</f>
+        <f t="shared" si="9"/>
         <v>14157.500793650001</v>
       </c>
       <c r="I42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.15750079365</v>
       </c>
       <c r="K42" s="1">
-        <f>B42/$H42*100</f>
+        <f t="shared" si="10"/>
         <v>96.203420353039405</v>
       </c>
       <c r="L42" s="1">
-        <f>C42/$H42*100</f>
+        <f t="shared" si="11"/>
         <v>0.57319999364858376</v>
       </c>
       <c r="M42" s="1">
-        <f>D42/$H42*100</f>
+        <f t="shared" si="12"/>
         <v>0.39943490609136401</v>
       </c>
       <c r="N42" s="1">
-        <f>E42/$H42*100</f>
+        <f t="shared" si="13"/>
         <v>2.7413030425120848</v>
       </c>
       <c r="O42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8705878762569611E-2</v>
       </c>
       <c r="P42" s="1">
-        <f>G42/$H42*100</f>
+        <f t="shared" si="14"/>
         <v>4.3935825945988466E-2</v>
       </c>
     </row>
@@ -18391,39 +18391,39 @@
       <c r="F43">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G43" s="18">
+      <c r="G43" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H43">
-        <f>SUM(B43:G43)</f>
+        <f t="shared" si="9"/>
         <v>14157.500793650001</v>
       </c>
       <c r="I43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.15750079365</v>
       </c>
       <c r="K43" s="1">
-        <f>B43/$H43*100</f>
+        <f t="shared" si="10"/>
         <v>96.203420353039405</v>
       </c>
       <c r="L43" s="1">
-        <f>C43/$H43*100</f>
+        <f t="shared" si="11"/>
         <v>0.57319999364858376</v>
       </c>
       <c r="M43" s="1">
-        <f>D43/$H43*100</f>
+        <f t="shared" si="12"/>
         <v>0.39943490609136401</v>
       </c>
       <c r="N43" s="1">
-        <f>E43/$H43*100</f>
+        <f t="shared" si="13"/>
         <v>2.7413030425120848</v>
       </c>
       <c r="O43" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8705878762569611E-2</v>
       </c>
       <c r="P43" s="1">
-        <f>G43/$H43*100</f>
+        <f t="shared" si="14"/>
         <v>4.3935825945988466E-2</v>
       </c>
     </row>
@@ -18446,39 +18446,39 @@
       <c r="F44">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G44" s="18">
+      <c r="G44" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H44">
-        <f>SUM(B44:G44)</f>
+        <f t="shared" si="9"/>
         <v>14157.500793650001</v>
       </c>
       <c r="I44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.15750079365</v>
       </c>
       <c r="K44" s="1">
-        <f>B44/$H44*100</f>
+        <f t="shared" si="10"/>
         <v>96.203420353039405</v>
       </c>
       <c r="L44" s="1">
-        <f>C44/$H44*100</f>
+        <f t="shared" si="11"/>
         <v>0.57319999364858376</v>
       </c>
       <c r="M44" s="1">
-        <f>D44/$H44*100</f>
+        <f t="shared" si="12"/>
         <v>0.39943490609136401</v>
       </c>
       <c r="N44" s="1">
-        <f>E44/$H44*100</f>
+        <f t="shared" si="13"/>
         <v>2.7413030425120848</v>
       </c>
       <c r="O44" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8705878762569611E-2</v>
       </c>
       <c r="P44" s="1">
-        <f>G44/$H44*100</f>
+        <f t="shared" si="14"/>
         <v>4.3935825945988466E-2</v>
       </c>
     </row>
@@ -18501,39 +18501,39 @@
       <c r="F45">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G45" s="18">
+      <c r="G45" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H45">
-        <f>SUM(B45:G45)</f>
+        <f t="shared" si="9"/>
         <v>14157.500793650001</v>
       </c>
       <c r="I45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.15750079365</v>
       </c>
       <c r="K45" s="1">
-        <f>B45/$H45*100</f>
+        <f t="shared" si="10"/>
         <v>96.203420353039405</v>
       </c>
       <c r="L45" s="1">
-        <f>C45/$H45*100</f>
+        <f t="shared" si="11"/>
         <v>0.57319999364858376</v>
       </c>
       <c r="M45" s="1">
-        <f>D45/$H45*100</f>
+        <f t="shared" si="12"/>
         <v>0.39943490609136401</v>
       </c>
       <c r="N45" s="1">
-        <f>E45/$H45*100</f>
+        <f t="shared" si="13"/>
         <v>2.7413030425120848</v>
       </c>
       <c r="O45" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8705878762569611E-2</v>
       </c>
       <c r="P45" s="1">
-        <f>G45/$H45*100</f>
+        <f t="shared" si="14"/>
         <v>4.3935825945988466E-2</v>
       </c>
     </row>
@@ -18556,39 +18556,39 @@
       <c r="F46">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G46" s="18">
+      <c r="G46" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H46">
-        <f>SUM(B46:G46)</f>
+        <f t="shared" si="9"/>
         <v>14076.35</v>
       </c>
       <c r="I46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.07635</v>
       </c>
       <c r="K46" s="1">
-        <f>B46/$H46*100</f>
+        <f t="shared" si="10"/>
         <v>96.758037417370275</v>
       </c>
       <c r="L46" s="1">
-        <f>C46/$H46*100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M46" s="1">
-        <f>D46/$H46*100</f>
+        <f t="shared" si="12"/>
         <v>0.40173766636947783</v>
       </c>
       <c r="N46" s="1">
-        <f>E46/$H46*100</f>
+        <f t="shared" si="13"/>
         <v>2.7571067783907051</v>
       </c>
       <c r="O46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8929019902176343E-2</v>
       </c>
       <c r="P46" s="1">
-        <f>G46/$H46*100</f>
+        <f t="shared" si="14"/>
         <v>4.4189117967370801E-2</v>
       </c>
     </row>
@@ -18611,39 +18611,39 @@
       <c r="F47">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G47" s="18">
+      <c r="G47" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H47">
-        <f>SUM(B47:G47)</f>
+        <f t="shared" si="9"/>
         <v>14076.35</v>
       </c>
       <c r="I47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.07635</v>
       </c>
       <c r="K47" s="1">
-        <f>B47/$H47*100</f>
+        <f t="shared" si="10"/>
         <v>96.758037417370275</v>
       </c>
       <c r="L47" s="1">
-        <f>C47/$H47*100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M47" s="1">
-        <f>D47/$H47*100</f>
+        <f t="shared" si="12"/>
         <v>0.40173766636947783</v>
       </c>
       <c r="N47" s="1">
-        <f>E47/$H47*100</f>
+        <f t="shared" si="13"/>
         <v>2.7571067783907051</v>
       </c>
       <c r="O47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8929019902176343E-2</v>
       </c>
       <c r="P47" s="1">
-        <f>G47/$H47*100</f>
+        <f t="shared" si="14"/>
         <v>4.4189117967370801E-2</v>
       </c>
     </row>
@@ -18666,39 +18666,39 @@
       <c r="F48">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G48" s="18">
+      <c r="G48" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H48">
-        <f>SUM(B48:G48)</f>
+        <f t="shared" si="9"/>
         <v>14076.35</v>
       </c>
       <c r="I48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.07635</v>
       </c>
       <c r="K48" s="1">
-        <f>B48/$H48*100</f>
+        <f t="shared" si="10"/>
         <v>96.758037417370275</v>
       </c>
       <c r="L48" s="1">
-        <f>C48/$H48*100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M48" s="1">
-        <f>D48/$H48*100</f>
+        <f t="shared" si="12"/>
         <v>0.40173766636947783</v>
       </c>
       <c r="N48" s="1">
-        <f>E48/$H48*100</f>
+        <f t="shared" si="13"/>
         <v>2.7571067783907051</v>
       </c>
       <c r="O48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8929019902176343E-2</v>
       </c>
       <c r="P48" s="1">
-        <f>G48/$H48*100</f>
+        <f t="shared" si="14"/>
         <v>4.4189117967370801E-2</v>
       </c>
     </row>
@@ -18721,39 +18721,39 @@
       <c r="F49">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G49" s="18">
+      <c r="G49" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H49">
-        <f>SUM(B49:G49)</f>
+        <f t="shared" si="9"/>
         <v>14076.35</v>
       </c>
       <c r="I49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.07635</v>
       </c>
       <c r="K49" s="1">
-        <f>B49/$H49*100</f>
+        <f t="shared" si="10"/>
         <v>96.758037417370275</v>
       </c>
       <c r="L49" s="1">
-        <f>C49/$H49*100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M49" s="1">
-        <f>D49/$H49*100</f>
+        <f t="shared" si="12"/>
         <v>0.40173766636947783</v>
       </c>
       <c r="N49" s="1">
-        <f>E49/$H49*100</f>
+        <f t="shared" si="13"/>
         <v>2.7571067783907051</v>
       </c>
       <c r="O49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8929019902176343E-2</v>
       </c>
       <c r="P49" s="1">
-        <f>G49/$H49*100</f>
+        <f t="shared" si="14"/>
         <v>4.4189117967370801E-2</v>
       </c>
     </row>
@@ -18776,39 +18776,39 @@
       <c r="F50">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G50" s="18">
+      <c r="G50" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H50">
-        <f>SUM(B50:G50)</f>
+        <f t="shared" si="9"/>
         <v>14076.35</v>
       </c>
       <c r="I50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.07635</v>
       </c>
       <c r="K50" s="1">
-        <f>B50/$H50*100</f>
+        <f t="shared" si="10"/>
         <v>96.758037417370275</v>
       </c>
       <c r="L50" s="1">
-        <f>C50/$H50*100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M50" s="1">
-        <f>D50/$H50*100</f>
+        <f t="shared" si="12"/>
         <v>0.40173766636947783</v>
       </c>
       <c r="N50" s="1">
-        <f>E50/$H50*100</f>
+        <f t="shared" si="13"/>
         <v>2.7571067783907051</v>
       </c>
       <c r="O50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8929019902176343E-2</v>
       </c>
       <c r="P50" s="1">
-        <f>G50/$H50*100</f>
+        <f t="shared" si="14"/>
         <v>4.4189117967370801E-2</v>
       </c>
     </row>
@@ -18831,39 +18831,39 @@
       <c r="F51">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G51" s="18">
+      <c r="G51" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H51">
-        <f>SUM(B51:G51)</f>
+        <f t="shared" si="9"/>
         <v>14076.35</v>
       </c>
       <c r="I51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.07635</v>
       </c>
       <c r="K51" s="1">
-        <f>B51/$H51*100</f>
+        <f t="shared" si="10"/>
         <v>96.758037417370275</v>
       </c>
       <c r="L51" s="1">
-        <f>C51/$H51*100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M51" s="1">
-        <f>D51/$H51*100</f>
+        <f t="shared" si="12"/>
         <v>0.40173766636947783</v>
       </c>
       <c r="N51" s="1">
-        <f>E51/$H51*100</f>
+        <f t="shared" si="13"/>
         <v>2.7571067783907051</v>
       </c>
       <c r="O51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8929019902176343E-2</v>
       </c>
       <c r="P51" s="1">
-        <f>G51/$H51*100</f>
+        <f t="shared" si="14"/>
         <v>4.4189117967370801E-2</v>
       </c>
     </row>
@@ -18886,39 +18886,39 @@
       <c r="F52">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G52" s="18">
+      <c r="G52" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H52">
-        <f>SUM(B52:G52)</f>
+        <f t="shared" si="9"/>
         <v>14076.35</v>
       </c>
       <c r="I52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.07635</v>
       </c>
       <c r="K52" s="1">
-        <f>B52/$H52*100</f>
+        <f t="shared" si="10"/>
         <v>96.758037417370275</v>
       </c>
       <c r="L52" s="1">
-        <f>C52/$H52*100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M52" s="1">
-        <f>D52/$H52*100</f>
+        <f t="shared" si="12"/>
         <v>0.40173766636947783</v>
       </c>
       <c r="N52" s="1">
-        <f>E52/$H52*100</f>
+        <f t="shared" si="13"/>
         <v>2.7571067783907051</v>
       </c>
       <c r="O52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8929019902176343E-2</v>
       </c>
       <c r="P52" s="1">
-        <f>G52/$H52*100</f>
+        <f t="shared" si="14"/>
         <v>4.4189117967370801E-2</v>
       </c>
     </row>
@@ -18941,39 +18941,39 @@
       <c r="F53">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G53" s="18">
+      <c r="G53" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H53">
-        <f>SUM(B53:G53)</f>
+        <f t="shared" si="9"/>
         <v>14076.35</v>
       </c>
       <c r="I53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.07635</v>
       </c>
       <c r="K53" s="1">
-        <f>B53/$H53*100</f>
+        <f t="shared" si="10"/>
         <v>96.758037417370275</v>
       </c>
       <c r="L53" s="1">
-        <f>C53/$H53*100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M53" s="1">
-        <f>D53/$H53*100</f>
+        <f t="shared" si="12"/>
         <v>0.40173766636947783</v>
       </c>
       <c r="N53" s="1">
-        <f>E53/$H53*100</f>
+        <f t="shared" si="13"/>
         <v>2.7571067783907051</v>
       </c>
       <c r="O53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8929019902176343E-2</v>
       </c>
       <c r="P53" s="1">
-        <f>G53/$H53*100</f>
+        <f t="shared" si="14"/>
         <v>4.4189117967370801E-2</v>
       </c>
     </row>
@@ -18996,39 +18996,39 @@
       <c r="F54">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G54" s="18">
+      <c r="G54" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H54">
-        <f>SUM(B54:G54)</f>
+        <f t="shared" si="9"/>
         <v>14076.35</v>
       </c>
       <c r="I54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.07635</v>
       </c>
       <c r="K54" s="1">
-        <f>B54/$H54*100</f>
+        <f t="shared" si="10"/>
         <v>96.758037417370275</v>
       </c>
       <c r="L54" s="1">
-        <f>C54/$H54*100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M54" s="1">
-        <f>D54/$H54*100</f>
+        <f t="shared" si="12"/>
         <v>0.40173766636947783</v>
       </c>
       <c r="N54" s="1">
-        <f>E54/$H54*100</f>
+        <f t="shared" si="13"/>
         <v>2.7571067783907051</v>
       </c>
       <c r="O54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8929019902176343E-2</v>
       </c>
       <c r="P54" s="1">
-        <f>G54/$H54*100</f>
+        <f t="shared" si="14"/>
         <v>4.4189117967370801E-2</v>
       </c>
     </row>
@@ -19051,39 +19051,39 @@
       <c r="F55">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G55" s="18">
+      <c r="G55" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H55">
-        <f>SUM(B55:G55)</f>
+        <f t="shared" si="9"/>
         <v>14076.35</v>
       </c>
       <c r="I55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.07635</v>
       </c>
       <c r="K55" s="1">
-        <f>B55/$H55*100</f>
+        <f t="shared" si="10"/>
         <v>96.758037417370275</v>
       </c>
       <c r="L55" s="1">
-        <f>C55/$H55*100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M55" s="1">
-        <f>D55/$H55*100</f>
+        <f t="shared" si="12"/>
         <v>0.40173766636947783</v>
       </c>
       <c r="N55" s="1">
-        <f>E55/$H55*100</f>
+        <f t="shared" si="13"/>
         <v>2.7571067783907051</v>
       </c>
       <c r="O55" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8929019902176343E-2</v>
       </c>
       <c r="P55" s="1">
-        <f>G55/$H55*100</f>
+        <f t="shared" si="14"/>
         <v>4.4189117967370801E-2</v>
       </c>
     </row>
@@ -19106,39 +19106,39 @@
       <c r="F56">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G56" s="18">
+      <c r="G56" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H56">
-        <f>SUM(B56:G56)</f>
+        <f t="shared" si="9"/>
         <v>14076.35</v>
       </c>
       <c r="I56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.07635</v>
       </c>
       <c r="K56" s="1">
-        <f>B56/$H56*100</f>
+        <f t="shared" si="10"/>
         <v>96.758037417370275</v>
       </c>
       <c r="L56" s="1">
-        <f>C56/$H56*100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M56" s="1">
-        <f>D56/$H56*100</f>
+        <f t="shared" si="12"/>
         <v>0.40173766636947783</v>
       </c>
       <c r="N56" s="1">
-        <f>E56/$H56*100</f>
+        <f t="shared" si="13"/>
         <v>2.7571067783907051</v>
       </c>
       <c r="O56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8929019902176343E-2</v>
       </c>
       <c r="P56" s="1">
-        <f>G56/$H56*100</f>
+        <f t="shared" si="14"/>
         <v>4.4189117967370801E-2</v>
       </c>
     </row>
@@ -19161,39 +19161,39 @@
       <c r="F57">
         <v>5.4797850930000003</v>
       </c>
-      <c r="G57" s="18">
+      <c r="G57" s="16">
         <v>6.2202149069999999</v>
       </c>
       <c r="H57">
-        <f>SUM(B57:G57)</f>
+        <f t="shared" si="9"/>
         <v>14076.35</v>
       </c>
       <c r="I57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14.07635</v>
       </c>
       <c r="K57" s="1">
-        <f>B57/$H57*100</f>
+        <f t="shared" si="10"/>
         <v>96.758037417370275</v>
       </c>
       <c r="L57" s="1">
-        <f>C57/$H57*100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M57" s="1">
-        <f>D57/$H57*100</f>
+        <f t="shared" si="12"/>
         <v>0.40173766636947783</v>
       </c>
       <c r="N57" s="1">
-        <f>E57/$H57*100</f>
+        <f t="shared" si="13"/>
         <v>2.7571067783907051</v>
       </c>
       <c r="O57" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8929019902176343E-2</v>
       </c>
       <c r="P57" s="1">
-        <f>G57/$H57*100</f>
+        <f t="shared" si="14"/>
         <v>4.4189117967370801E-2</v>
       </c>
     </row>
@@ -19226,7 +19226,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -19243,7 +19243,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="17"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>

</xml_diff>